<commit_message>
pcb lib updated, connectors added
</commit_message>
<xml_diff>
--- a/info/orders.xlsx
+++ b/info/orders.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FE4A9-D338-4140-9175-C572A93FA7FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="3510" windowWidth="12885" windowHeight="6645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="3510" windowWidth="12885" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>NAU8810</t>
   </si>
@@ -49,8 +48,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,27 +187,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,24 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -433,20 +396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B5:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -454,7 +418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -462,7 +426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -470,7 +434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -478,34 +442,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="link" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C11" r:id="rId3" xr:uid="{5AF06D69-EF03-43C4-85EC-5E911BA69692}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{62CB0378-388D-4700-ABE1-3043C9D07610}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{2867EC7B-6195-4FDB-9217-053880CCDC54}"/>
+    <hyperlink ref="C5" r:id="rId1" display="link"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C11" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="D13" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -513,12 +481,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>